<commit_message>
fix input of subject code bug
</commit_message>
<xml_diff>
--- a/db/data.xlsx
+++ b/db/data.xlsx
@@ -89,9 +89,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -109,91 +109,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,9 +132,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,7 +208,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,7 +223,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,6 +236,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -262,13 +262,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +406,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,157 +436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,12 +456,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -478,6 +491,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,15 +530,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -525,21 +540,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -556,148 +556,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
let user know each entered character is right or wrong
</commit_message>
<xml_diff>
--- a/db/data.xlsx
+++ b/db/data.xlsx
@@ -1,41 +1,477 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="1"/>
+  </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
     <sheet name="experimentData" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+  <si>
+    <t>Subject Code</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Word Frequency</t>
+  </si>
+  <si>
+    <t>Reference Structure</t>
+  </si>
+  <si>
+    <t>Trial Time</t>
+  </si>
+  <si>
+    <t>Error Rate</t>
+  </si>
+  <si>
+    <t>Character Times</t>
+  </si>
+  <si>
+    <t>targetStrings</t>
+  </si>
+  <si>
+    <t>中国淡水鱼之王白</t>
+  </si>
+  <si>
+    <t>朱婷自白初进国家</t>
+  </si>
+  <si>
+    <t>美国威胁袭击伊朗</t>
+  </si>
+  <si>
+    <t>在阿里能熬十年的</t>
+  </si>
+  <si>
+    <t>wordFrequencyLevels</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>referenceStructureLevels</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>simplified</t>
+  </si>
+  <si>
+    <t>balancedLatinSquare(wf, rs)</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>totalBlock</t>
+  </si>
+  <si>
+    <t>warmUpStrings</t>
+  </si>
+  <si>
+    <t>您吃了吗</t>
+  </si>
+  <si>
+    <t>天气不错</t>
+  </si>
+  <si>
+    <t>恭喜发财</t>
+  </si>
+  <si>
+    <t>夜黑风高</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -43,18 +479,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,44 +1104,54 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="17.125" customWidth="1"/>
+    <col min="10" max="10" width="10.375" customWidth="1"/>
+    <col min="11" max="11" width="9.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Subject Code</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Block</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Trial</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Word Frequency</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Reference Structure</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Trial Time</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Error Rate</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Character Times</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2">
         <v>1</v>
       </c>
@@ -434,49 +1174,49 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>3310.7550000004267</v>
+        <v>3310.75500000043</v>
       </c>
       <c r="I2">
-        <v>4495.530000000144</v>
+        <v>4495.53000000014</v>
       </c>
       <c r="J2">
-        <v>10912.02499999963</v>
+        <v>10912.0249999996</v>
       </c>
       <c r="K2">
-        <v>6367.285000000265</v>
+        <v>6367.28500000027</v>
       </c>
       <c r="L2">
-        <v>1759.6000000012282</v>
+        <v>1759.60000000123</v>
       </c>
       <c r="M2">
-        <v>4177.009999999427</v>
+        <v>4177.00999999943</v>
       </c>
       <c r="N2">
-        <v>4439.404999999169</v>
+        <v>4439.40499999917</v>
       </c>
       <c r="O2">
-        <v>3231.995000000097</v>
+        <v>3231.9950000001</v>
       </c>
       <c r="P2">
-        <v>34063.640000000305</v>
+        <v>34063.6400000003</v>
       </c>
       <c r="Q2">
-        <v>3535.775000000285</v>
+        <v>3535.77500000029</v>
       </c>
       <c r="R2">
         <v>4143.17999999912</v>
       </c>
       <c r="S2">
-        <v>12063.38499999947</v>
+        <v>12063.3849999995</v>
       </c>
       <c r="T2">
-        <v>2807.614999999714</v>
+        <v>2807.61499999971</v>
       </c>
       <c r="U2">
-        <v>5032.6550000008865</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>5032.65500000089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>1</v>
       </c>
@@ -499,49 +1239,49 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>11118.760000001232</v>
+        <v>11118.7600000012</v>
       </c>
       <c r="I3">
-        <v>10167.165000000736</v>
+        <v>10167.1650000007</v>
       </c>
       <c r="J3">
-        <v>6631.299999999086</v>
+        <v>6631.29999999909</v>
       </c>
       <c r="K3">
-        <v>3399.7650000001013</v>
+        <v>3399.7650000001</v>
       </c>
       <c r="L3">
-        <v>12343.450000000303</v>
+        <v>12343.4500000003</v>
       </c>
       <c r="M3">
-        <v>2248.050000000163</v>
+        <v>2248.05000000016</v>
       </c>
       <c r="N3">
-        <v>4039.960000000079</v>
+        <v>4039.96000000008</v>
       </c>
       <c r="O3">
-        <v>2759.495000000228</v>
+        <v>2759.49500000023</v>
       </c>
       <c r="P3">
-        <v>5360.704999999143</v>
+        <v>5360.70499999914</v>
       </c>
       <c r="Q3">
-        <v>7015.660000000964</v>
+        <v>7015.66000000096</v>
       </c>
       <c r="R3">
-        <v>5840.244999999413</v>
+        <v>5840.24499999941</v>
       </c>
       <c r="S3">
-        <v>2623.4499999991385</v>
+        <v>2623.44999999914</v>
       </c>
       <c r="T3">
-        <v>2335.3499999993946</v>
+        <v>2335.34999999939</v>
       </c>
       <c r="U3">
         <v>7567.78500000108</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>1</v>
       </c>
@@ -561,52 +1301,52 @@
         <v>342890</v>
       </c>
       <c r="G4">
-        <v>0.21428571428571427</v>
+        <v>0.214285714285714</v>
       </c>
       <c r="H4">
         <v>4896.27499999915</v>
       </c>
       <c r="I4">
-        <v>4574.9849999992875</v>
+        <v>4574.98499999929</v>
       </c>
       <c r="J4">
-        <v>22064.010000000068</v>
+        <v>22064.0100000001</v>
       </c>
       <c r="K4">
-        <v>41416.139999999374</v>
+        <v>41416.1399999994</v>
       </c>
       <c r="L4">
-        <v>47960.39000000019</v>
+        <v>47960.3900000002</v>
       </c>
       <c r="M4">
-        <v>36175.30500000069</v>
+        <v>36175.3050000007</v>
       </c>
       <c r="N4">
-        <v>13976.384999999893</v>
+        <v>13976.3849999999</v>
       </c>
       <c r="O4">
-        <v>7655.805000000342</v>
+        <v>7655.80500000034</v>
       </c>
       <c r="P4">
-        <v>2592.3099999999977</v>
+        <v>2592.31</v>
       </c>
       <c r="Q4">
         <v>8578.84500000003</v>
       </c>
       <c r="R4">
-        <v>4775.534999998868</v>
+        <v>4775.53499999887</v>
       </c>
       <c r="S4">
-        <v>3391.9399999995367</v>
+        <v>3391.93999999954</v>
       </c>
       <c r="T4">
-        <v>62416.479999999865</v>
+        <v>62416.4799999999</v>
       </c>
       <c r="U4">
         <v>45223.9150000005</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>1</v>
       </c>
@@ -629,49 +1369,49 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>3590.995000000461</v>
+        <v>3590.99500000046</v>
       </c>
       <c r="I5">
-        <v>4023.499999999418</v>
+        <v>4023.49999999942</v>
       </c>
       <c r="J5">
-        <v>2504.1849999997066</v>
+        <v>2504.18499999971</v>
       </c>
       <c r="K5">
-        <v>2999.4050000004936</v>
+        <v>2999.40500000049</v>
       </c>
       <c r="L5">
-        <v>6496.159999998868</v>
+        <v>6496.15999999887</v>
       </c>
       <c r="M5">
-        <v>11239.775000000023</v>
+        <v>11239.775</v>
       </c>
       <c r="N5">
-        <v>3879.734999998589</v>
+        <v>3879.73499999859</v>
       </c>
       <c r="O5">
-        <v>2334.8399999995017</v>
+        <v>2334.8399999995</v>
       </c>
       <c r="P5">
-        <v>6815.475000001257</v>
+        <v>6815.47500000126</v>
       </c>
       <c r="Q5">
-        <v>4663.305000000051</v>
+        <v>4663.30500000005</v>
       </c>
       <c r="R5">
-        <v>2918.0300000007264</v>
+        <v>2918.03000000073</v>
       </c>
       <c r="S5">
-        <v>2174.7099999992643</v>
+        <v>2174.70999999926</v>
       </c>
       <c r="T5">
-        <v>51617.41499999876</v>
+        <v>51617.4149999988</v>
       </c>
       <c r="U5">
-        <v>16224.334999999031</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>16224.334999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>1</v>
       </c>
@@ -694,49 +1434,49 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>3272.3249999999534</v>
+        <v>3272.32499999995</v>
       </c>
       <c r="I6">
-        <v>4495.030000000028</v>
+        <v>4495.03000000003</v>
       </c>
       <c r="J6">
-        <v>12366.475000000675</v>
+        <v>12366.4750000007</v>
       </c>
       <c r="K6">
-        <v>7919.1300000002375</v>
+        <v>7919.13000000024</v>
       </c>
       <c r="L6">
-        <v>8886.539999999572</v>
+        <v>8886.53999999957</v>
       </c>
       <c r="M6">
-        <v>4214.884999999311</v>
+        <v>4214.88499999931</v>
       </c>
       <c r="N6">
-        <v>4775.215000001481</v>
+        <v>4775.21500000148</v>
       </c>
       <c r="O6">
-        <v>2958.4949999989476</v>
+        <v>2958.49499999895</v>
       </c>
       <c r="P6">
-        <v>18167.054999999935</v>
+        <v>18167.0549999999</v>
       </c>
       <c r="Q6">
-        <v>1703.2500000004657</v>
+        <v>1703.25000000047</v>
       </c>
       <c r="R6">
-        <v>12015.069999999483</v>
+        <v>12015.0699999995</v>
       </c>
       <c r="S6">
-        <v>11785.055000000284</v>
+        <v>11785.0550000003</v>
       </c>
       <c r="T6">
         <v>2910.89500000095</v>
       </c>
       <c r="U6">
-        <v>5150.864999999641</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>5150.86499999964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>1</v>
       </c>
@@ -759,49 +1499,49 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>11695.080000001355</v>
+        <v>11695.0800000014</v>
       </c>
       <c r="I7">
-        <v>10983.529999999446</v>
+        <v>10983.5299999994</v>
       </c>
       <c r="J7">
-        <v>6775.569999999716</v>
+        <v>6775.56999999972</v>
       </c>
       <c r="K7">
-        <v>3088.1699999991106</v>
+        <v>3088.16999999911</v>
       </c>
       <c r="L7">
-        <v>25470.16500000062</v>
+        <v>25470.1650000006</v>
       </c>
       <c r="M7">
-        <v>2719.4149999995716</v>
+        <v>2719.41499999957</v>
       </c>
       <c r="N7">
-        <v>4615.569999999949</v>
+        <v>4615.56999999995</v>
       </c>
       <c r="O7">
-        <v>3838.6700000009732</v>
+        <v>3838.67000000097</v>
       </c>
       <c r="P7">
-        <v>4439.229999999981</v>
+        <v>4439.22999999998</v>
       </c>
       <c r="Q7">
-        <v>8240.674999999115</v>
+        <v>8240.67499999912</v>
       </c>
       <c r="R7">
-        <v>6094.820000000298</v>
+        <v>6094.8200000003</v>
       </c>
       <c r="S7">
-        <v>2710.9450000007637</v>
+        <v>2710.94500000076</v>
       </c>
       <c r="T7">
-        <v>2279.575000000419</v>
+        <v>2279.57500000042</v>
       </c>
       <c r="U7">
-        <v>8566.310000000172</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>8566.31000000017</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>1</v>
       </c>
@@ -821,52 +1561,52 @@
         <v>245832</v>
       </c>
       <c r="G8">
-        <v>0.21428571428571427</v>
+        <v>0.214285714285714</v>
       </c>
       <c r="H8">
-        <v>5063.344999998575</v>
+        <v>5063.34499999858</v>
       </c>
       <c r="I8">
-        <v>4311.2950000013225</v>
+        <v>4311.29500000132</v>
       </c>
       <c r="J8">
-        <v>15151.620000000577</v>
+        <v>15151.6200000006</v>
       </c>
       <c r="K8">
-        <v>15015.260000000242</v>
+        <v>15015.2600000002</v>
       </c>
       <c r="L8">
-        <v>22999.120000000577</v>
+        <v>22999.1200000006</v>
       </c>
       <c r="M8">
-        <v>7254.989999999525</v>
+        <v>7254.98999999953</v>
       </c>
       <c r="N8">
-        <v>26311.54500000039</v>
+        <v>26311.5450000004</v>
       </c>
       <c r="O8">
-        <v>7863.820000000531</v>
+        <v>7863.82000000053</v>
       </c>
       <c r="P8">
-        <v>2630.9400000008754</v>
+        <v>2630.94000000088</v>
       </c>
       <c r="Q8">
-        <v>8567.365000000922</v>
+        <v>8567.36500000092</v>
       </c>
       <c r="R8">
-        <v>5711.405000000028</v>
+        <v>5711.40500000003</v>
       </c>
       <c r="S8">
         <v>8592.20499999891</v>
       </c>
       <c r="T8">
-        <v>43095.47999999998</v>
+        <v>43095.48</v>
       </c>
       <c r="U8">
-        <v>50326.67500000028</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>50326.6750000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>1</v>
       </c>
@@ -889,49 +1629,49 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>2127.7800000007264</v>
+        <v>2127.78000000073</v>
       </c>
       <c r="I9">
-        <v>3959.495000001043</v>
+        <v>3959.49500000104</v>
       </c>
       <c r="J9">
-        <v>2382.884999999078</v>
+        <v>2382.88499999908</v>
       </c>
       <c r="K9">
-        <v>2703.3600000012666</v>
+        <v>2703.36000000127</v>
       </c>
       <c r="L9">
-        <v>9469.965000000084</v>
+        <v>9469.96500000008</v>
       </c>
       <c r="M9">
-        <v>12071.680000000866</v>
+        <v>12071.6800000009</v>
       </c>
       <c r="N9">
-        <v>2575.2599999995437</v>
+        <v>2575.25999999954</v>
       </c>
       <c r="O9">
-        <v>2255.4149999998044</v>
+        <v>2255.4149999998</v>
       </c>
       <c r="P9">
-        <v>14694.620000000112</v>
+        <v>14694.6200000001</v>
       </c>
       <c r="Q9">
-        <v>3550.9999999993015</v>
+        <v>3550.9999999993</v>
       </c>
       <c r="R9">
-        <v>2583.0149999982677</v>
+        <v>2583.01499999827</v>
       </c>
       <c r="S9">
-        <v>2047.2349999998696</v>
+        <v>2047.23499999987</v>
       </c>
       <c r="T9">
-        <v>13230.099999998929</v>
+        <v>13230.0999999989</v>
       </c>
       <c r="U9">
-        <v>16191.784999998985</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>16191.784999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>1</v>
       </c>
@@ -954,49 +1694,49 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>2464.7100000001956</v>
+        <v>2464.7100000002</v>
       </c>
       <c r="I10">
-        <v>4390.959999998799</v>
+        <v>4390.9599999988</v>
       </c>
       <c r="J10">
-        <v>11551.545000000391</v>
+        <v>11551.5450000004</v>
       </c>
       <c r="K10">
-        <v>8126.174999999581</v>
+        <v>8126.17499999958</v>
       </c>
       <c r="L10">
-        <v>8527.050000000745</v>
+        <v>8527.05000000075</v>
       </c>
       <c r="M10">
-        <v>4751.744999999646</v>
+        <v>4751.74499999965</v>
       </c>
       <c r="N10">
-        <v>4455.590000001248</v>
+        <v>4455.59000000125</v>
       </c>
       <c r="O10">
-        <v>7487.089999998687</v>
+        <v>7487.08999999869</v>
       </c>
       <c r="P10">
-        <v>5790.610000000102</v>
+        <v>5790.6100000001</v>
       </c>
       <c r="Q10">
-        <v>1558.8050000006333</v>
+        <v>1558.80500000063</v>
       </c>
       <c r="R10">
-        <v>1918.8899999989662</v>
+        <v>1918.88999999897</v>
       </c>
       <c r="S10">
-        <v>1390.9650000005495</v>
+        <v>1390.96500000055</v>
       </c>
       <c r="T10">
-        <v>1159.2450000005774</v>
+        <v>1159.24500000058</v>
       </c>
       <c r="U10">
-        <v>1215.655000000028</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1215.65500000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1016,52 +1756,52 @@
         <v>25115</v>
       </c>
       <c r="G11">
-        <v>0.07142857142857142</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="H11">
-        <v>1703.1999999999534</v>
+        <v>1703.19999999995</v>
       </c>
       <c r="I11">
-        <v>1455.0799999998417</v>
+        <v>1455.07999999984</v>
       </c>
       <c r="J11">
-        <v>1039.399999999674</v>
+        <v>1039.39999999967</v>
       </c>
       <c r="K11">
-        <v>1271.2300000002142</v>
+        <v>1271.23000000021</v>
       </c>
       <c r="L11">
-        <v>1638.5449999999255</v>
+        <v>1638.54499999993</v>
       </c>
       <c r="M11">
-        <v>1253.8649999985937</v>
+        <v>1253.86499999859</v>
       </c>
       <c r="N11">
-        <v>1358.9100000008475</v>
+        <v>1358.91000000085</v>
       </c>
       <c r="O11">
-        <v>1063.4499999997206</v>
+        <v>1063.44999999972</v>
       </c>
       <c r="P11">
-        <v>1262.7100000006612</v>
+        <v>1262.71000000066</v>
       </c>
       <c r="Q11">
-        <v>911.4500000013504</v>
+        <v>911.45000000135</v>
       </c>
       <c r="R11">
-        <v>1143.2750000003725</v>
+        <v>1143.27500000037</v>
       </c>
       <c r="S11">
-        <v>1039.679999999702</v>
+        <v>1039.6799999997</v>
       </c>
       <c r="T11">
-        <v>774.3950000004843</v>
+        <v>774.395000000484</v>
       </c>
       <c r="U11">
-        <v>1871.1500000008382</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1871.15000000084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1081,52 +1821,52 @@
         <v>47789</v>
       </c>
       <c r="G12">
-        <v>0.6428571428571429</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="H12">
-        <v>1414.5500000012107</v>
+        <v>1414.55000000121</v>
       </c>
       <c r="I12">
         <v>1256.22999999905</v>
       </c>
       <c r="J12">
-        <v>13326.660000000615</v>
+        <v>13326.6600000006</v>
       </c>
       <c r="K12">
-        <v>3574.214999998687</v>
+        <v>3574.21499999869</v>
       </c>
       <c r="L12">
-        <v>1222.2700000002515</v>
+        <v>1222.27000000025</v>
       </c>
       <c r="M12">
-        <v>1582.9850000010338</v>
+        <v>1582.98500000103</v>
       </c>
       <c r="N12">
-        <v>2144.435000000056</v>
+        <v>2144.43500000006</v>
       </c>
       <c r="O12">
         <v>2074.44000000041</v>
       </c>
       <c r="P12">
-        <v>1982.8649999999907</v>
+        <v>1982.86499999999</v>
       </c>
       <c r="Q12">
-        <v>1478.989999999525</v>
+        <v>1478.98999999953</v>
       </c>
       <c r="R12">
-        <v>1815.5399999995716</v>
+        <v>1815.53999999957</v>
       </c>
       <c r="S12">
-        <v>1991.4850000003353</v>
+        <v>1991.48500000034</v>
       </c>
       <c r="T12">
-        <v>1225.7250000000931</v>
+        <v>1225.72500000009</v>
       </c>
       <c r="U12">
-        <v>446.22499999962747</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>446.224999999627</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1149,49 +1889,49 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1141.9900000002235</v>
+        <v>1141.99000000022</v>
       </c>
       <c r="I13">
-        <v>911.7050000003073</v>
+        <v>911.705000000307</v>
       </c>
       <c r="J13">
-        <v>822.2150000000838</v>
+        <v>822.215000000084</v>
       </c>
       <c r="K13">
-        <v>705.8799999994226</v>
+        <v>705.879999999423</v>
       </c>
       <c r="L13">
-        <v>714.4850000003353</v>
+        <v>714.485000000335</v>
       </c>
       <c r="M13">
-        <v>1367.1149999992922</v>
+        <v>1367.11499999929</v>
       </c>
       <c r="N13">
-        <v>1206.609999999404</v>
+        <v>1206.6099999994</v>
       </c>
       <c r="O13">
-        <v>565.1899999994785</v>
+        <v>565.189999999478</v>
       </c>
       <c r="P13">
-        <v>1887.1049999997485</v>
+        <v>1887.10499999975</v>
       </c>
       <c r="Q13">
         <v>1156.35499999905</v>
       </c>
       <c r="R13">
-        <v>767.4499999992549</v>
+        <v>767.449999999255</v>
       </c>
       <c r="S13">
-        <v>470.8999999985099</v>
+        <v>470.89999999851</v>
       </c>
       <c r="T13">
-        <v>1231.1700000010896</v>
+        <v>1231.17000000109</v>
       </c>
       <c r="U13">
-        <v>2982.564999998547</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>2982.56499999855</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1214,49 +1954,49 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>983.2450000012759</v>
+        <v>983.245000001276</v>
       </c>
       <c r="I14">
         <v>910.149999999674</v>
       </c>
       <c r="J14">
-        <v>1829.9900000002235</v>
+        <v>1829.99000000022</v>
       </c>
       <c r="K14">
         <v>974.285000000149</v>
       </c>
       <c r="L14">
-        <v>3559.9700000004377</v>
+        <v>3559.97000000044</v>
       </c>
       <c r="M14">
-        <v>664.8399999993853</v>
+        <v>664.839999999385</v>
       </c>
       <c r="N14">
-        <v>1279.3199999995995</v>
+        <v>1279.3199999996</v>
       </c>
       <c r="O14">
-        <v>1115.4799999985844</v>
+        <v>1115.47999999858</v>
       </c>
       <c r="P14">
-        <v>5295.135000000242</v>
+        <v>5295.13500000024</v>
       </c>
       <c r="Q14">
-        <v>919.1449999997858</v>
+        <v>919.144999999786</v>
       </c>
       <c r="R14">
-        <v>3302.5550000001676</v>
+        <v>3302.55500000017</v>
       </c>
       <c r="S14">
-        <v>1374.9299999999348</v>
+        <v>1374.92999999993</v>
       </c>
       <c r="T14">
-        <v>1015.3150000006426</v>
+        <v>1015.31500000064</v>
       </c>
       <c r="U14">
-        <v>919.8799999994226</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>919.879999999423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1279,49 +2019,49 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1190.3399999991525</v>
+        <v>1190.33999999915</v>
       </c>
       <c r="I15">
-        <v>1423.2499999997672</v>
+        <v>1423.24999999977</v>
       </c>
       <c r="J15">
-        <v>990.8450000004377</v>
+        <v>990.845000000438</v>
       </c>
       <c r="K15">
-        <v>1182.704999999376</v>
+        <v>1182.70499999938</v>
       </c>
       <c r="L15">
-        <v>1662.589999999851</v>
+        <v>1662.58999999985</v>
       </c>
       <c r="M15">
-        <v>799.3750000004657</v>
+        <v>799.375000000466</v>
       </c>
       <c r="N15">
-        <v>1271.634999999078</v>
+        <v>1271.63499999908</v>
       </c>
       <c r="O15">
-        <v>1247.559999999823</v>
+        <v>1247.55999999982</v>
       </c>
       <c r="P15">
-        <v>1086.3300000000745</v>
+        <v>1086.33000000007</v>
       </c>
       <c r="Q15">
-        <v>1191.1899999994785</v>
+        <v>1191.18999999948</v>
       </c>
       <c r="R15">
-        <v>1398.7900000012014</v>
+        <v>1398.7900000012</v>
       </c>
       <c r="S15">
-        <v>863.8750000009313</v>
+        <v>863.875000000931</v>
       </c>
       <c r="T15">
         <v>879.055000001099</v>
       </c>
       <c r="U15">
-        <v>1608.2500000009313</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1608.25000000093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1341,52 +2081,52 @@
         <v>51291</v>
       </c>
       <c r="G16">
-        <v>0.14285714285714285</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="H16">
-        <v>1348.9399999999441</v>
+        <v>1348.93999999994</v>
       </c>
       <c r="I16">
-        <v>1223.219999999972</v>
+        <v>1223.21999999997</v>
       </c>
       <c r="J16">
-        <v>2487.565000001341</v>
+        <v>2487.56500000134</v>
       </c>
       <c r="K16">
-        <v>4871.520000000717</v>
+        <v>4871.52000000072</v>
       </c>
       <c r="L16">
-        <v>2904.9249999988824</v>
+        <v>2904.92499999888</v>
       </c>
       <c r="M16">
-        <v>3303.570000000065</v>
+        <v>3303.57000000007</v>
       </c>
       <c r="N16">
         <v>3671.06500000041</v>
       </c>
       <c r="O16">
-        <v>2983.8199999993667</v>
+        <v>2983.81999999937</v>
       </c>
       <c r="P16">
-        <v>1159.8549999999814</v>
+        <v>1159.85499999998</v>
       </c>
       <c r="Q16">
-        <v>1920.1800000008661</v>
+        <v>1920.18000000087</v>
       </c>
       <c r="R16">
-        <v>1446.5200000014156</v>
+        <v>1446.52000000142</v>
       </c>
       <c r="S16">
-        <v>2503.029999999795</v>
+        <v>2503.0299999998</v>
       </c>
       <c r="T16">
-        <v>4032.010000000708</v>
+        <v>4032.01000000071</v>
       </c>
       <c r="U16">
-        <v>9366.830000001006</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>9366.83000000101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1409,200 +2149,211 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>851.0649999990128</v>
+        <v>851.064999999013</v>
       </c>
       <c r="I17">
-        <v>1510.720000000205</v>
+        <v>1510.7200000002</v>
       </c>
       <c r="J17">
         <v>871.054999999702</v>
       </c>
       <c r="K17">
-        <v>1326.1349999993108</v>
+        <v>1326.13499999931</v>
       </c>
       <c r="L17">
-        <v>1000.0149999996647</v>
+        <v>1000.01499999966</v>
       </c>
       <c r="M17">
-        <v>1439.2650000008289</v>
+        <v>1439.26500000083</v>
       </c>
       <c r="N17">
-        <v>1289.2599999995437</v>
+        <v>1289.25999999954</v>
       </c>
       <c r="O17">
-        <v>552.7899999995716</v>
+        <v>552.789999999572</v>
       </c>
       <c r="P17">
-        <v>1647.1099999998696</v>
+        <v>1647.10999999987</v>
       </c>
       <c r="Q17">
-        <v>1208.2150000005495</v>
+        <v>1208.21500000055</v>
       </c>
       <c r="R17">
-        <v>1110.8100000000559</v>
+        <v>1110.81000000006</v>
       </c>
       <c r="S17">
-        <v>654.7499999995343</v>
+        <v>654.749999999534</v>
       </c>
       <c r="T17">
-        <v>2111.1499999987427</v>
+        <v>2111.14999999874</v>
       </c>
       <c r="U17">
-        <v>3839.254999998957</v>
+        <v>3839.25499999896</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:U17"/>
+    <ignoredError sqref="A1:U17" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="4" width="31.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>targetStrings</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>中国淡水鱼之王白鲟被宣布灭绝</v>
-      </c>
-      <c r="B2" t="str">
-        <v>朱婷自白初进国家队时曾被看衰</v>
-      </c>
-      <c r="C2" t="str">
-        <v>美国威胁袭击伊朗古代文化遗址</v>
-      </c>
-      <c r="D2" t="str">
-        <v>在阿里能熬十年的员工都是宝贝</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>wordFrequencyLevels</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>random</v>
-      </c>
-      <c r="B5" t="str">
-        <v>high</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>referenceStructureLevels</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>whole</v>
-      </c>
-      <c r="B8" t="str">
-        <v>simplified</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>balancedLatinSquare(wf, rs)</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>0,0</v>
-      </c>
-      <c r="B11" t="str">
-        <v>0,1</v>
-      </c>
-      <c r="C11" t="str">
-        <v>1,1</v>
-      </c>
-      <c r="D11" t="str">
-        <v>1,0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>0,1</v>
-      </c>
-      <c r="B12" t="str">
-        <v>1,0</v>
-      </c>
-      <c r="C12" t="str">
-        <v>0,0</v>
-      </c>
-      <c r="D12" t="str">
-        <v>1,1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>1,0</v>
-      </c>
-      <c r="B13" t="str">
-        <v>1,1</v>
-      </c>
-      <c r="C13" t="str">
-        <v>0,1</v>
-      </c>
-      <c r="D13" t="str">
-        <v>0,0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>1,1</v>
-      </c>
-      <c r="B14" t="str">
-        <v>0,0</v>
-      </c>
-      <c r="C14" t="str">
-        <v>1,0</v>
-      </c>
-      <c r="D14" t="str">
-        <v>0,1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>totalBlock</v>
-      </c>
-    </row>
-    <row r="17">
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17">
         <v>3</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>warmUpStrings</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>您吃了吗</v>
-      </c>
-      <c r="B20" t="str">
-        <v>天气不错</v>
-      </c>
-      <c r="C20" t="str">
-        <v>恭喜发财</v>
-      </c>
-      <c r="D20" t="str">
-        <v>夜黑风高</v>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D20"/>
+    <ignoredError sqref="A1:D1 A3:D20" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>